<commit_message>
added the input() function in translator.c and updated the log file
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CA4D74-10E9-420B-A5AB-0B7E909A3CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBEA907-CD02-4059-A75B-81CDEE4D5D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>~10 min</t>
   </si>
@@ -47,6 +47,9 @@
     <t>~2 hrs</t>
   </si>
   <si>
+    <t>~3 hrs</t>
+  </si>
+  <si>
     <t>plan.c - Google Docs</t>
   </si>
   <si>
@@ -129,6 +132,9 @@
   </si>
   <si>
     <t>added the error() function and changed the name from converter to translator since that reflects it better. Needed to do some more research in the git commit issues</t>
+  </si>
+  <si>
+    <t>Completed the translator scanning portion and tested it using a temp printing function. Corrected some bugs related to the scanning.</t>
   </si>
 </sst>
 </file>
@@ -522,10 +528,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,19 +546,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -573,13 +580,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -587,16 +594,16 @@
         <v>45221</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -604,10 +611,10 @@
         <v>45221</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -616,10 +623,10 @@
         <v>45225</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -627,10 +634,10 @@
         <v>45226</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,10 +645,10 @@
         <v>45228</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,13 +656,13 @@
         <v>45231</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -663,10 +670,10 @@
         <v>45232</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -674,10 +681,10 @@
         <v>45232</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -685,10 +692,26 @@
         <v>45233</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45234</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the input() function to translator.c additionally the helper functions get_data_type and add_to_stream were as helper functions to input and eventually output. Header functions were added to io.h and will be written next. added the -Wall flag to the Makefile for compiling
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBEA907-CD02-4059-A75B-81CDEE4D5D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74E009E-714E-4622-B72E-EECF299FDF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>~10 min</t>
   </si>
@@ -74,9 +74,6 @@
     <t>yisroelshulman/auto_grader: A Program that can auto evaluate simple programs. (github.com)</t>
   </si>
   <si>
-    <t>The repo is currently private</t>
-  </si>
-  <si>
     <t>&lt; 5 min</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>~ 5 hrs</t>
   </si>
   <si>
-    <t>added the error() function and changed the name from converter to translator since that reflects it better</t>
-  </si>
-  <si>
     <t>~ 1 hr</t>
   </si>
   <si>
@@ -135,6 +129,18 @@
   </si>
   <si>
     <t>Completed the translator scanning portion and tested it using a temp printing function. Corrected some bugs related to the scanning.</t>
+  </si>
+  <si>
+    <t>~3hrs</t>
+  </si>
+  <si>
+    <t>coded part of the translator that translates the .sul files into the IO test cases.</t>
+  </si>
+  <si>
+    <t>~4 hrs</t>
+  </si>
+  <si>
+    <t>completing the slide deck for the deliverable</t>
   </si>
 </sst>
 </file>
@@ -528,11 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,13 +586,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -594,16 +600,13 @@
         <v>45221</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,10 +614,10 @@
         <v>45221</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -623,10 +626,10 @@
         <v>45225</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -634,10 +637,10 @@
         <v>45226</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -645,10 +648,10 @@
         <v>45228</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,13 +659,13 @@
         <v>45231</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -670,10 +673,10 @@
         <v>45232</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -681,10 +684,10 @@
         <v>45232</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -692,10 +695,10 @@
         <v>45233</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -706,12 +709,29 @@
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45235</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45236</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the code for the output() function and ran a short test to make sure it works
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74E009E-714E-4622-B72E-EECF299FDF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1908AC3-ED9E-490D-88F4-BB064CFA774F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>~10 min</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>completing the slide deck for the deliverable</t>
+  </si>
+  <si>
+    <t>finished coding the input portion of the io and tested it.</t>
+  </si>
+  <si>
+    <t>~3.5 hrs</t>
   </si>
 </sst>
 </file>
@@ -534,11 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,6 +740,17 @@
         <v>34</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45237</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>

<commit_message>
fixed the buffer overflow of the write_stream function in io.c
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1908AC3-ED9E-490D-88F4-BB064CFA774F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098421A6-0061-494F-A4D8-54D6DF82F4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>~10 min</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>~3.5 hrs</t>
+  </si>
+  <si>
+    <t>~1hr</t>
+  </si>
+  <si>
+    <t>commenting the translator.c and .h files</t>
   </si>
 </sst>
 </file>
@@ -540,11 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +757,17 @@
         <v>35</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45238</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>

<commit_message>
added the print_result function, still need to complete the print_case_result() function
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16DA60-AF12-46E2-B871-A778523CE9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74CF519-F769-4F1A-97B0-566FCBA8EAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>~10 min</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>commenting the translator.c and .h files</t>
+  </si>
+  <si>
+    <t>redesigned some of the plan and moved around and commented some more code</t>
+  </si>
+  <si>
+    <t>cleaned up the code by moving around functions and adding the crx.c and .h files. Also had a 40 min meeting with Professor Weiss about TuringCraft</t>
+  </si>
+  <si>
+    <t>~1 hr</t>
+  </si>
+  <si>
+    <t>looked into and wrote a small extention for vs code to do syntax highlighting for .sul files. Thank you documentation and the "yo generator-code" tool</t>
+  </si>
+  <si>
+    <t>~3-4 hrs</t>
   </si>
 </sst>
 </file>
@@ -546,11 +561,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,6 +783,39 @@
         <v>38</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45243</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45244</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42689</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>

<commit_message>
commented the crx.c and crx.h files
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74CF519-F769-4F1A-97B0-566FCBA8EAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01D32FA-B099-435B-BDBD-329CCC3DF011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>~10 min</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>~3-4 hrs</t>
+  </si>
+  <si>
+    <t>added the syntax highlighter, fixed some issues with negative numbers, and finished the print result section</t>
   </si>
 </sst>
 </file>
@@ -561,11 +564,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,6 +819,22 @@
         <v>42</v>
       </c>
     </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45246</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45247</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>

<commit_message>
commented the io.c and io.h files
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01D32FA-B099-435B-BDBD-329CCC3DF011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303ABCCF-9FD1-4DFE-89ED-1FC419D142CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>~10 min</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>added the syntax highlighter, fixed some issues with negative numbers, and finished the print result section</t>
+  </si>
+  <si>
+    <t>wrote the comparators and fixed the crx functions. Completed the memory management for the io and results. Fixed the bug where runtime errors would cause the program to segfault. Added comments to files.</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,9 +833,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45247</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the menu.c and menu.h files and default menu. currently the selections are just options that print the selection
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303ABCCF-9FD1-4DFE-89ED-1FC419D142CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0913451-D809-4C45-AE9B-ACCBEFB41BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>~10 min</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>wrote the comparators and fixed the crx functions. Completed the memory management for the io and results. Fixed the bug where runtime errors would cause the program to segfault. Added comments to files.</t>
+  </si>
+  <si>
+    <t>Commented the io and crx files and worked on the documentation</t>
+  </si>
+  <si>
+    <t>~2hrs</t>
+  </si>
+  <si>
+    <t>Worked more on the documentation</t>
   </si>
 </sst>
 </file>
@@ -567,11 +576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,6 +853,28 @@
         <v>45</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45248</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45249</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>

<commit_message>
added the checks functionality to the program and tested it. seems to work
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0913451-D809-4C45-AE9B-ACCBEFB41BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7113A9A-8C77-4F7C-AB7E-5D4B49C1A60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>~10 min</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Worked more on the documentation</t>
+  </si>
+  <si>
+    <t>~5 hrs</t>
+  </si>
+  <si>
+    <t>added the menu and the controller that handles most of the program logic</t>
   </si>
 </sst>
 </file>
@@ -576,11 +582,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,6 +881,17 @@
         <v>48</v>
       </c>
     </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45250</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>

<commit_message>
added the instructions for the sum_ints_m_to_n program
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\projects\auto_grader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7113A9A-8C77-4F7C-AB7E-5D4B49C1A60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C39F830-4D14-4459-A3EA-A80F491447E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{18199C19-A4EB-47CD-89B5-DD3B66B464D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>~10 min</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>added the menu and the controller that handles most of the program logic</t>
+  </si>
+  <si>
+    <t>~1 hrs</t>
+  </si>
+  <si>
+    <t>added the dubgger and moved the debugging functions to debug.c</t>
+  </si>
+  <si>
+    <t>looked into how to display the files and settled to make the program specific to linux distributoins and use the less  command to show the files. Fixed an error that when multiple errors are in a .sul file the program would seg fault.</t>
+  </si>
+  <si>
+    <t>added the problem list and the instructions</t>
   </si>
 </sst>
 </file>
@@ -582,11 +594,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E54CB90-DC39-415B-B537-C786D6DE7DE5}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,6 +904,39 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45253</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45254</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45255</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="heading=h.7k4osnrxhg6p" display="https://docs.google.com/document/d/1ViXbkssAJwmKOazD73EiH6vF_gwntnEDwdpoQPGfn9M/edit - heading=h.7k4osnrxhg6p" xr:uid="{0E4D3381-E024-4D1A-A83B-047DF8EE5F55}"/>

</xml_diff>